<commit_message>
rspec parties_controller new test passed
</commit_message>
<xml_diff>
--- a/contributions-summary-by-a1724402.xlsx
+++ b/contributions-summary-by-a1724402.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Dropbox\UNI\2019 SEM 1\SaaS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danlu\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55432F6-B360-4C14-8283-9E8CD89E6A57}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contributions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>Contributions Assessed by:</t>
   </si>
@@ -113,9 +120,6 @@
     <t>Max</t>
   </si>
   <si>
-    <t>Alfred</t>
-  </si>
-  <si>
     <t>Aiman</t>
   </si>
   <si>
@@ -132,12 +136,30 @@
   </si>
   <si>
     <t>Haven't heard anything about his contribution</t>
+  </si>
+  <si>
+    <t>Styling for parties list and adding testing</t>
+  </si>
+  <si>
+    <t>Worked on reviewing and fitting git pull requests</t>
+  </si>
+  <si>
+    <t>Potential drag and drop feature for voting</t>
+  </si>
+  <si>
+    <t>Created voting method for above and low the line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assisting with basic functionality </t>
+  </si>
+  <si>
+    <t>Xuxin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -578,23 +600,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="75.625" customWidth="1"/>
+    <col min="4" max="4" width="75.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -606,7 +628,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -615,13 +637,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -635,7 +657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>23</v>
       </c>
@@ -646,10 +668,10 @@
         <v>11</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
@@ -660,10 +682,10 @@
         <v>9</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
@@ -674,49 +696,49 @@
         <v>11</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="17"/>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
@@ -730,7 +752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="str">
         <f>A6</f>
         <v>a1724402</v>
@@ -739,10 +761,14 @@
         <f>B6</f>
         <v>Dan</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="str">
         <f t="shared" ref="A15:B15" si="0">A7</f>
         <v>a1DDDDDDD</v>
@@ -751,10 +777,14 @@
         <f t="shared" si="0"/>
         <v>Parthey</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="str">
         <f t="shared" ref="A16:B16" si="1">A8</f>
         <v>a1DDDDDDD</v>
@@ -763,22 +793,30 @@
         <f t="shared" si="1"/>
         <v>Max</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="str">
         <f t="shared" ref="A17:B17" si="2">A9</f>
         <v>a1DDDDDDD</v>
       </c>
       <c r="B17" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>Alfred</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
-    </row>
-    <row r="18" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <f>B9</f>
+        <v>Xuxin</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="12" t="str">
         <f t="shared" ref="A18:B18" si="3">A10</f>
         <v>a1DDDDDDD</v>
@@ -787,21 +825,25 @@
         <f t="shared" si="3"/>
         <v>Aiman</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
       <c r="C19" s="17"/>
       <c r="D19" s="18"/>
     </row>
-    <row r="20" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
         <v>2</v>
       </c>
@@ -815,7 +857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="str">
         <f t="shared" ref="A22:B22" si="4">A14</f>
         <v>a1724402</v>
@@ -827,7 +869,7 @@
       <c r="C22" s="10"/>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="str">
         <f t="shared" ref="A23:B23" si="5">A15</f>
         <v>a1DDDDDDD</v>
@@ -839,7 +881,7 @@
       <c r="C23" s="10"/>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="str">
         <f t="shared" ref="A24:B24" si="6">A16</f>
         <v>a1DDDDDDD</v>
@@ -851,19 +893,19 @@
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="str">
         <f t="shared" ref="A25:B25" si="7">A17</f>
         <v>a1DDDDDDD</v>
       </c>
       <c r="B25" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>Alfred</v>
+        <v>Xuxin</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="11"/>
     </row>
-    <row r="26" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="12" t="str">
         <f t="shared" ref="A26:B26" si="8">A18</f>
         <v>a1DDDDDDD</v>
@@ -875,18 +917,18 @@
       <c r="C26" s="14"/>
       <c r="D26" s="15"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
       <c r="C27" s="17"/>
       <c r="D27" s="18"/>
     </row>
-    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
         <v>2</v>
       </c>
@@ -900,7 +942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="str">
         <f t="shared" ref="A30:B30" si="9">A22</f>
         <v>a1724402</v>
@@ -912,7 +954,7 @@
       <c r="C30" s="10"/>
       <c r="D30" s="11"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="str">
         <f t="shared" ref="A31:B31" si="10">A23</f>
         <v>a1DDDDDDD</v>
@@ -924,7 +966,7 @@
       <c r="C31" s="10"/>
       <c r="D31" s="11"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="str">
         <f t="shared" ref="A32:B32" si="11">A24</f>
         <v>a1DDDDDDD</v>
@@ -936,19 +978,19 @@
       <c r="C32" s="10"/>
       <c r="D32" s="11"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="str">
         <f t="shared" ref="A33:B33" si="12">A25</f>
         <v>a1DDDDDDD</v>
       </c>
       <c r="B33" s="9" t="str">
         <f t="shared" si="12"/>
-        <v>Alfred</v>
+        <v>Xuxin</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="11"/>
     </row>
-    <row r="34" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="12" t="str">
         <f t="shared" ref="A34:B34" si="13">A26</f>
         <v>a1DDDDDDD</v>
@@ -960,12 +1002,12 @@
       <c r="C34" s="14"/>
       <c r="D34" s="15"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B36" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B37" s="2" t="s">
         <v>8</v>
       </c>
@@ -973,7 +1015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B38" s="2" t="s">
         <v>10</v>
       </c>
@@ -981,7 +1023,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B39" s="2" t="s">
         <v>12</v>
       </c>
@@ -989,7 +1031,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B40" s="2" t="s">
         <v>14</v>
       </c>
@@ -997,7 +1039,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B41" s="2" t="s">
         <v>16</v>
       </c>
@@ -1005,7 +1047,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B42" s="2" t="s">
         <v>18</v>
       </c>

</xml_diff>